<commit_message>
Updated game plan and added 5th day of data
</commit_message>
<xml_diff>
--- a/Estimator_Worksheet.xlsx
+++ b/Estimator_Worksheet.xlsx
@@ -8,20 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kijah\Documents\Data_Bootcamp\Estimator_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7940B528-AE87-47B3-9AB2-43CB6763DAF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B749ACB-04EF-4FC5-9F0E-0E29FE778A61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6105" yWindow="-16320" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary - Rates" sheetId="1" r:id="rId1"/>
     <sheet name="Summary - Table" sheetId="2" r:id="rId2"/>
     <sheet name="Conduit + Wire - Pricing Calcul" sheetId="3" r:id="rId3"/>
     <sheet name="Conduit + Wire - Table" sheetId="4" r:id="rId4"/>
-    <sheet name="Working_Table" sheetId="6" r:id="rId5"/>
-    <sheet name="Cleaned_Data" sheetId="7" r:id="rId6"/>
+    <sheet name="Working_Table" sheetId="5" r:id="rId5"/>
+    <sheet name="Cleaned_Data" sheetId="6" r:id="rId6"/>
+    <sheet name="Working_Table1" sheetId="7" r:id="rId7"/>
+    <sheet name="Cleaned_Data1" sheetId="8" r:id="rId8"/>
+    <sheet name="Working_Table2" sheetId="9" r:id="rId9"/>
+    <sheet name="Cleaned_Data2" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -39,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="130">
   <si>
     <t>Sales Tax</t>
   </si>
@@ -348,6 +351,87 @@
   </si>
   <si>
     <t>https://www.cooper-electric.com/product/detail/23760/thhn-copper-wic-thhn-10-str-blk-500r</t>
+  </si>
+  <si>
+    <t>10/23/2022 23:33:41</t>
+  </si>
+  <si>
+    <t>https://www.homedepot.com/p/Halex-3-4-in-Electric-Metallic-Tube-EMT-Set-Screw-Coupling-5-Pack-26282/202288508</t>
+  </si>
+  <si>
+    <t>3/4 in. Electrical Metallic Tube (EMT) Set-Screw Connector (5-Pack)</t>
+  </si>
+  <si>
+    <t>https://www.homedepot.com/p/Halex-3-4-in-Electrical-Metallic-Tube-EMT-Set-Screw-Connectors-5-Pack-26272/100163157</t>
+  </si>
+  <si>
+    <t>1 in. Electrical Metallic Tube (EMT) Set-Screw Connector</t>
+  </si>
+  <si>
+    <t>https://www.homedepot.com/p/Halex-1-in-Electrical-Metallic-Tube-EMT-Set-Screw-Connector-62710/100562217</t>
+  </si>
+  <si>
+    <t>https://www.dkhardware.com/southwire-250-ft-12-2-solid-romex-simpull-cu-nm-b-w-g-wire-28828255-product-3154834.html</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/b/12-3-Romex/92078/bn_7023293830</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Cerrowire-112-4201J-500-Feet-Stranded-Black/dp/B00D49VU6W</t>
+  </si>
+  <si>
+    <t>https://www.homedepot.com/p/1-in-x-10-ft-Electric-Metallic-Tube-EMT-Conduit-101568/100400409</t>
+  </si>
+  <si>
+    <t>https://www.wilmar.com/Sku/24-87610/allied-tube-and-conduit-1-in-x-10-ft-electric-metallic-tube-emt-conduit-091111020032-101568</t>
+  </si>
+  <si>
+    <t>truevalue</t>
+  </si>
+  <si>
+    <t>https://www.truevalue.com/emt-conduit-steel-thinwall-1-in-x-10-ft</t>
+  </si>
+  <si>
+    <t>https://www.supplyworks.com/Sku/202077151/halex-12-in-electrical-metallic-tube-emt-set-screw-coupling-5-pack-051411232207-23220</t>
+  </si>
+  <si>
+    <t>https://www.lowes.com/pd/Sigma-Electric-ProConnex-1-2-in-Set-Screw-Coupling-Electrical-Metal-Tubing-Compatible-Conduit-Fitting/1100263</t>
+  </si>
+  <si>
+    <t>https://www.lowes.com/pd/Halex-3-4-in-EMT-STEEL-SET-SCREW-CONNECTOR-5-BAG/1002846668</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/itm/363478081520</t>
+  </si>
+  <si>
+    <t>landmsupply</t>
+  </si>
+  <si>
+    <t>https://www.landmsupply.com/southwire-romex-simpull-cable-w-ground-white-14-2-awg-250-ft-28827455</t>
+  </si>
+  <si>
+    <t>https://www.lowes.com/pd/Southwire-Romex-SIMpull-250-ft-12-2-Non-Metallic-Wire-By-the-Roll/1193433</t>
+  </si>
+  <si>
+    <t>https://www.homedepot.com/p/Southwire-500-ft-6-Black-Stranded-CU-SIMpull-THHN-Wire-20493301/202316339</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/p/1700352648</t>
+  </si>
+  <si>
+    <t>10/24/2022 14:10:34</t>
+  </si>
+  <si>
+    <t>https://www.supplyworks.com/Sku/202328185/halex-34-in-electrical-metallic-tube-emt-set-screw-coupling-5-pack-051411232221-23222</t>
+  </si>
+  <si>
+    <t>superarbor</t>
+  </si>
+  <si>
+    <t>https://www.superarbor.io/products/100163157-3-4-in-electrical-metallic-tube-emt-set-screw-connectors-5-pack</t>
+  </si>
+  <si>
+    <t>https://www.homedepot.com/p/Southwire-250-ft-14-2-Romex-SIMpull-Solid-NM-B-W-G-Wire-28827469/202019377</t>
   </si>
 </sst>
 </file>
@@ -358,7 +442,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -514,6 +598,16 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -583,7 +677,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -838,12 +932,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -965,14 +1089,37 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="17" fillId="11" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -985,23 +1132,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1292,6 +1422,7 @@
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="27.46484375" customWidth="1"/>
+    <col min="2" max="2" width="9.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -1335,6 +1466,1046 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:F51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="2.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.9296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="119.1328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.86328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B1" s="72" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="72" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="72" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="72" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="72">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2">
+        <v>7.22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="72">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3">
+        <v>7.68</v>
+      </c>
+      <c r="D3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="72">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4">
+        <v>5.88</v>
+      </c>
+      <c r="D4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="72">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5">
+        <v>9.09</v>
+      </c>
+      <c r="D5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" t="s">
+        <v>124</v>
+      </c>
+      <c r="F5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="72">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6">
+        <v>11.91</v>
+      </c>
+      <c r="D6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="72">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7">
+        <v>10.47</v>
+      </c>
+      <c r="D7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="72">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8">
+        <v>8.36</v>
+      </c>
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="72">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9">
+        <v>98.99</v>
+      </c>
+      <c r="D9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="72">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10">
+        <v>20.62</v>
+      </c>
+      <c r="D10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" t="s">
+        <v>112</v>
+      </c>
+      <c r="F10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="72">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11">
+        <v>17.55</v>
+      </c>
+      <c r="D11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E11" t="s">
+        <v>113</v>
+      </c>
+      <c r="F11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" s="72">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12">
+        <v>8.9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>82</v>
+      </c>
+      <c r="E12" t="s">
+        <v>83</v>
+      </c>
+      <c r="F12" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" s="72">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13">
+        <v>24.99</v>
+      </c>
+      <c r="D13" t="s">
+        <v>114</v>
+      </c>
+      <c r="E13" t="s">
+        <v>115</v>
+      </c>
+      <c r="F13" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" s="72">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14">
+        <v>3.98</v>
+      </c>
+      <c r="D14" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" t="s">
+        <v>86</v>
+      </c>
+      <c r="F14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" s="72">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15">
+        <v>5.99</v>
+      </c>
+      <c r="D15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" s="72">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16">
+        <v>2.1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>87</v>
+      </c>
+      <c r="E16" t="s">
+        <v>88</v>
+      </c>
+      <c r="F16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17" s="72">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17">
+        <v>5.99</v>
+      </c>
+      <c r="D17" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" t="s">
+        <v>117</v>
+      </c>
+      <c r="F17" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18" s="72">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18">
+        <v>2.98</v>
+      </c>
+      <c r="D18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" t="s">
+        <v>104</v>
+      </c>
+      <c r="F18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19" s="72">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19">
+        <v>3.66</v>
+      </c>
+      <c r="D19" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" t="s">
+        <v>126</v>
+      </c>
+      <c r="F19" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20" s="72">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20">
+        <v>2.98</v>
+      </c>
+      <c r="D20" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" t="s">
+        <v>55</v>
+      </c>
+      <c r="F20" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A21" s="72">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21">
+        <v>3.6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>127</v>
+      </c>
+      <c r="E21" t="s">
+        <v>128</v>
+      </c>
+      <c r="F21" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A22" s="72">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="D22" t="s">
+        <v>57</v>
+      </c>
+      <c r="E22" t="s">
+        <v>58</v>
+      </c>
+      <c r="F22" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23" s="72">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23">
+        <v>3.98</v>
+      </c>
+      <c r="D23" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" t="s">
+        <v>86</v>
+      </c>
+      <c r="F23" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24" s="72">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24">
+        <v>5.99</v>
+      </c>
+      <c r="D24" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" t="s">
+        <v>52</v>
+      </c>
+      <c r="F24" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25" s="72">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25">
+        <v>5.99</v>
+      </c>
+      <c r="D25" t="s">
+        <v>76</v>
+      </c>
+      <c r="E25" t="s">
+        <v>89</v>
+      </c>
+      <c r="F25" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A26" s="72">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26">
+        <v>2.29</v>
+      </c>
+      <c r="D26" t="s">
+        <v>87</v>
+      </c>
+      <c r="E26" t="s">
+        <v>88</v>
+      </c>
+      <c r="F26" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A27" s="72">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>105</v>
+      </c>
+      <c r="C27">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D27" t="s">
+        <v>57</v>
+      </c>
+      <c r="E27" t="s">
+        <v>106</v>
+      </c>
+      <c r="F27" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A28" s="72">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>105</v>
+      </c>
+      <c r="C28">
+        <v>5.99</v>
+      </c>
+      <c r="D28" t="s">
+        <v>76</v>
+      </c>
+      <c r="E28" t="s">
+        <v>118</v>
+      </c>
+      <c r="F28" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29" s="72">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>107</v>
+      </c>
+      <c r="C29">
+        <v>1.6</v>
+      </c>
+      <c r="D29" t="s">
+        <v>57</v>
+      </c>
+      <c r="E29" t="s">
+        <v>108</v>
+      </c>
+      <c r="F29" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A30" s="72">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30">
+        <v>118</v>
+      </c>
+      <c r="D30" t="s">
+        <v>57</v>
+      </c>
+      <c r="E30" t="s">
+        <v>129</v>
+      </c>
+      <c r="F30" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A31" s="72">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31">
+        <v>114</v>
+      </c>
+      <c r="D31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E31" t="s">
+        <v>90</v>
+      </c>
+      <c r="F31" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A32" s="72">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32">
+        <v>111.99</v>
+      </c>
+      <c r="D32" t="s">
+        <v>65</v>
+      </c>
+      <c r="E32" t="s">
+        <v>119</v>
+      </c>
+      <c r="F32" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A33" s="72">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33">
+        <v>84.99</v>
+      </c>
+      <c r="D33" t="s">
+        <v>120</v>
+      </c>
+      <c r="E33" t="s">
+        <v>121</v>
+      </c>
+      <c r="F33" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A34" s="72">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34">
+        <v>158</v>
+      </c>
+      <c r="D34" t="s">
+        <v>57</v>
+      </c>
+      <c r="E34" t="s">
+        <v>63</v>
+      </c>
+      <c r="F34" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A35" s="72">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35">
+        <v>158</v>
+      </c>
+      <c r="D35" t="s">
+        <v>76</v>
+      </c>
+      <c r="E35" t="s">
+        <v>93</v>
+      </c>
+      <c r="F35" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A36" s="72">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36">
+        <v>149</v>
+      </c>
+      <c r="D36" t="s">
+        <v>57</v>
+      </c>
+      <c r="E36" t="s">
+        <v>94</v>
+      </c>
+      <c r="F36" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A37" s="72">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>64</v>
+      </c>
+      <c r="C37">
+        <v>149</v>
+      </c>
+      <c r="D37" t="s">
+        <v>76</v>
+      </c>
+      <c r="E37" t="s">
+        <v>122</v>
+      </c>
+      <c r="F37" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A38" s="72">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>64</v>
+      </c>
+      <c r="C38">
+        <v>200.02</v>
+      </c>
+      <c r="D38" t="s">
+        <v>84</v>
+      </c>
+      <c r="E38" t="s">
+        <v>109</v>
+      </c>
+      <c r="F38" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A39" s="72">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>67</v>
+      </c>
+      <c r="C39">
+        <v>289</v>
+      </c>
+      <c r="D39" t="s">
+        <v>57</v>
+      </c>
+      <c r="E39" t="s">
+        <v>68</v>
+      </c>
+      <c r="F39" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A40" s="72">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>67</v>
+      </c>
+      <c r="C40">
+        <v>279</v>
+      </c>
+      <c r="D40" t="s">
+        <v>76</v>
+      </c>
+      <c r="E40" t="s">
+        <v>95</v>
+      </c>
+      <c r="F40" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A41" s="72">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>67</v>
+      </c>
+      <c r="C41">
+        <v>315.01</v>
+      </c>
+      <c r="D41" t="s">
+        <v>65</v>
+      </c>
+      <c r="E41" t="s">
+        <v>110</v>
+      </c>
+      <c r="F41" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A42" s="72">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>67</v>
+      </c>
+      <c r="C42">
+        <v>339.09</v>
+      </c>
+      <c r="D42" t="s">
+        <v>96</v>
+      </c>
+      <c r="E42" t="s">
+        <v>97</v>
+      </c>
+      <c r="F42" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A43" s="72">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>69</v>
+      </c>
+      <c r="C43">
+        <v>765</v>
+      </c>
+      <c r="D43" t="s">
+        <v>57</v>
+      </c>
+      <c r="E43" t="s">
+        <v>98</v>
+      </c>
+      <c r="F43" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A44" s="72">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>69</v>
+      </c>
+      <c r="C44">
+        <v>613.64</v>
+      </c>
+      <c r="D44" t="s">
+        <v>49</v>
+      </c>
+      <c r="E44" t="s">
+        <v>70</v>
+      </c>
+      <c r="F44" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A45" s="72">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>69</v>
+      </c>
+      <c r="C45">
+        <v>1047.78</v>
+      </c>
+      <c r="D45" t="s">
+        <v>65</v>
+      </c>
+      <c r="E45" t="s">
+        <v>99</v>
+      </c>
+      <c r="F45" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A46" s="72">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>71</v>
+      </c>
+      <c r="C46">
+        <v>379</v>
+      </c>
+      <c r="D46" t="s">
+        <v>57</v>
+      </c>
+      <c r="E46" t="s">
+        <v>123</v>
+      </c>
+      <c r="F46" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A47" s="72">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C47">
+        <v>470.43</v>
+      </c>
+      <c r="D47" t="s">
+        <v>49</v>
+      </c>
+      <c r="E47" t="s">
+        <v>111</v>
+      </c>
+      <c r="F47" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A48" s="72">
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
+        <v>71</v>
+      </c>
+      <c r="C48">
+        <v>445.81</v>
+      </c>
+      <c r="D48" t="s">
+        <v>65</v>
+      </c>
+      <c r="E48" t="s">
+        <v>72</v>
+      </c>
+      <c r="F48" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A49" s="72">
+        <v>47</v>
+      </c>
+      <c r="B49" t="s">
+        <v>73</v>
+      </c>
+      <c r="C49">
+        <v>145</v>
+      </c>
+      <c r="D49" t="s">
+        <v>57</v>
+      </c>
+      <c r="E49" t="s">
+        <v>100</v>
+      </c>
+      <c r="F49" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A50" s="72">
+        <v>48</v>
+      </c>
+      <c r="B50" t="s">
+        <v>73</v>
+      </c>
+      <c r="C50">
+        <v>155.99</v>
+      </c>
+      <c r="D50" t="s">
+        <v>49</v>
+      </c>
+      <c r="E50" t="s">
+        <v>74</v>
+      </c>
+      <c r="F50" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A51" s="72">
+        <v>49</v>
+      </c>
+      <c r="B51" t="s">
+        <v>73</v>
+      </c>
+      <c r="C51">
+        <v>398.95</v>
+      </c>
+      <c r="D51" t="s">
+        <v>101</v>
+      </c>
+      <c r="E51" t="s">
+        <v>102</v>
+      </c>
+      <c r="F51" t="s">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1573,13 +2744,13 @@
       <c r="P8" s="63"/>
     </row>
     <row r="9" spans="1:16" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="81" t="s">
+      <c r="A9" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="72"/>
-      <c r="C9" s="72"/>
-      <c r="D9" s="72"/>
-      <c r="E9" s="82"/>
+      <c r="B9" s="74"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="74"/>
+      <c r="E9" s="75"/>
       <c r="F9" s="9"/>
       <c r="G9" s="51">
         <f t="shared" si="1"/>
@@ -1602,14 +2773,14 @@
         <v>11</v>
       </c>
       <c r="D10" s="14"/>
-      <c r="E10" s="83" t="s">
+      <c r="E10" s="76" t="s">
         <v>12</v>
       </c>
       <c r="F10" s="54" t="str">
         <f>C10</f>
         <v>TOTAL</v>
       </c>
-      <c r="G10" s="85" t="s">
+      <c r="G10" s="78" t="s">
         <v>13</v>
       </c>
       <c r="H10" s="63"/>
@@ -1629,11 +2800,11 @@
         <v>14</v>
       </c>
       <c r="D11" s="55"/>
-      <c r="E11" s="84"/>
+      <c r="E11" s="77"/>
       <c r="F11" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="74"/>
+      <c r="G11" s="79"/>
       <c r="H11" s="63"/>
       <c r="I11" s="63"/>
       <c r="J11" s="63"/>
@@ -1645,59 +2816,59 @@
       <c r="P11" s="63"/>
     </row>
     <row r="12" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="86" t="s">
+      <c r="A12" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="87">
+      <c r="B12" s="81">
         <f t="shared" ref="B12:G12" si="2">SUM(B2:B8)</f>
         <v>0</v>
       </c>
-      <c r="C12" s="87">
+      <c r="C12" s="81">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="D12" s="87">
+      <c r="D12" s="81">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E12" s="87">
+      <c r="E12" s="81">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F12" s="87">
+      <c r="F12" s="81">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G12" s="75">
+      <c r="G12" s="84">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H12" s="77" t="s">
+      <c r="H12" s="86" t="s">
         <v>17</v>
       </c>
-      <c r="I12" s="74"/>
-      <c r="J12" s="74"/>
-      <c r="K12" s="74"/>
-      <c r="L12" s="74"/>
-      <c r="M12" s="74"/>
+      <c r="I12" s="79"/>
+      <c r="J12" s="79"/>
+      <c r="K12" s="79"/>
+      <c r="L12" s="79"/>
+      <c r="M12" s="79"/>
       <c r="N12" s="63"/>
       <c r="O12" s="63"/>
       <c r="P12" s="63"/>
     </row>
     <row r="13" spans="1:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="74"/>
-      <c r="B13" s="74"/>
-      <c r="C13" s="74"/>
-      <c r="D13" s="74"/>
-      <c r="E13" s="74"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="76"/>
-      <c r="H13" s="78"/>
-      <c r="I13" s="74"/>
-      <c r="J13" s="74"/>
-      <c r="K13" s="74"/>
-      <c r="L13" s="74"/>
-      <c r="M13" s="74"/>
+      <c r="A13" s="79"/>
+      <c r="B13" s="79"/>
+      <c r="C13" s="79"/>
+      <c r="D13" s="79"/>
+      <c r="E13" s="79"/>
+      <c r="F13" s="79"/>
+      <c r="G13" s="85"/>
+      <c r="H13" s="87"/>
+      <c r="I13" s="79"/>
+      <c r="J13" s="79"/>
+      <c r="K13" s="79"/>
+      <c r="L13" s="79"/>
+      <c r="M13" s="79"/>
       <c r="N13" s="63"/>
       <c r="O13" s="63"/>
       <c r="P13" s="63"/>
@@ -1762,10 +2933,10 @@
       <c r="B18" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="79"/>
-      <c r="D18" s="80"/>
-      <c r="E18" s="80"/>
-      <c r="F18" s="80"/>
+      <c r="C18" s="88"/>
+      <c r="D18" s="89"/>
+      <c r="E18" s="89"/>
+      <c r="F18" s="89"/>
       <c r="G18" s="63"/>
       <c r="H18" s="63"/>
       <c r="I18" s="63"/>
@@ -1782,10 +2953,10 @@
       <c r="B19" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="71"/>
-      <c r="D19" s="72"/>
-      <c r="E19" s="72"/>
-      <c r="F19" s="72"/>
+      <c r="C19" s="82"/>
+      <c r="D19" s="74"/>
+      <c r="E19" s="74"/>
+      <c r="F19" s="74"/>
       <c r="G19" s="63"/>
       <c r="H19" s="63"/>
       <c r="I19" s="63"/>
@@ -1802,15 +2973,15 @@
       <c r="B20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="79"/>
-      <c r="D20" s="80"/>
-      <c r="E20" s="80"/>
-      <c r="F20" s="80"/>
-      <c r="G20" s="80"/>
-      <c r="H20" s="80"/>
-      <c r="I20" s="80"/>
-      <c r="J20" s="80"/>
-      <c r="K20" s="80"/>
+      <c r="C20" s="88"/>
+      <c r="D20" s="89"/>
+      <c r="E20" s="89"/>
+      <c r="F20" s="89"/>
+      <c r="G20" s="89"/>
+      <c r="H20" s="89"/>
+      <c r="I20" s="89"/>
+      <c r="J20" s="89"/>
+      <c r="K20" s="89"/>
       <c r="L20" s="63"/>
       <c r="M20" s="63"/>
       <c r="N20" s="63"/>
@@ -1822,10 +2993,10 @@
       <c r="B21" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="71"/>
-      <c r="D21" s="72"/>
-      <c r="E21" s="72"/>
-      <c r="F21" s="72"/>
+      <c r="C21" s="82"/>
+      <c r="D21" s="74"/>
+      <c r="E21" s="74"/>
+      <c r="F21" s="74"/>
       <c r="G21" s="67"/>
       <c r="H21" s="63"/>
       <c r="I21" s="63"/>
@@ -1855,14 +3026,14 @@
     <row r="23" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A23" s="63"/>
       <c r="B23" s="63"/>
-      <c r="C23" s="73" t="s">
+      <c r="C23" s="83" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="74"/>
-      <c r="E23" s="74"/>
-      <c r="F23" s="74"/>
-      <c r="G23" s="74"/>
-      <c r="H23" s="74"/>
+      <c r="D23" s="79"/>
+      <c r="E23" s="79"/>
+      <c r="F23" s="79"/>
+      <c r="G23" s="79"/>
+      <c r="H23" s="79"/>
       <c r="I23" s="63"/>
       <c r="J23" s="63"/>
       <c r="K23" s="63"/>
@@ -1875,12 +3046,12 @@
     <row r="24" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A24" s="63"/>
       <c r="B24" s="63"/>
-      <c r="C24" s="74"/>
-      <c r="D24" s="74"/>
-      <c r="E24" s="74"/>
-      <c r="F24" s="74"/>
-      <c r="G24" s="74"/>
-      <c r="H24" s="74"/>
+      <c r="C24" s="79"/>
+      <c r="D24" s="79"/>
+      <c r="E24" s="79"/>
+      <c r="F24" s="79"/>
+      <c r="G24" s="79"/>
+      <c r="H24" s="79"/>
       <c r="I24" s="63"/>
       <c r="J24" s="63"/>
       <c r="K24" s="63"/>
@@ -1893,12 +3064,12 @@
     <row r="25" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A25" s="63"/>
       <c r="B25" s="63"/>
-      <c r="C25" s="74"/>
-      <c r="D25" s="74"/>
-      <c r="E25" s="74"/>
-      <c r="F25" s="74"/>
-      <c r="G25" s="74"/>
-      <c r="H25" s="74"/>
+      <c r="C25" s="79"/>
+      <c r="D25" s="79"/>
+      <c r="E25" s="79"/>
+      <c r="F25" s="79"/>
+      <c r="G25" s="79"/>
+      <c r="H25" s="79"/>
       <c r="I25" s="63"/>
       <c r="J25" s="63"/>
       <c r="K25" s="63"/>
@@ -1928,6 +3099,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C23:H25"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:M13"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C20:K20"/>
     <mergeCell ref="A9:E9"/>
     <mergeCell ref="E10:E11"/>
     <mergeCell ref="G10:G11"/>
@@ -1937,13 +3115,6 @@
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="F12:F13"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C23:H25"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:M13"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="C20:K20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1953,7 +3124,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S51"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K8" sqref="K8"/>
     </sheetView>
@@ -2557,11 +3728,11 @@
         <v>1</v>
       </c>
       <c r="F34" s="7">
-        <f t="shared" ref="F34:F65" si="2">B34*(C34/E34)</f>
+        <f t="shared" ref="F34:F50" si="2">B34*(C34/E34)</f>
         <v>0</v>
       </c>
       <c r="H34">
-        <f t="shared" ref="H34:H65" si="3">B34*(G34/E34)</f>
+        <f t="shared" ref="H34:H50" si="3">B34*(G34/E34)</f>
         <v>0</v>
       </c>
     </row>
@@ -4022,7 +5193,7 @@
         <v>0</v>
       </c>
       <c r="D34" s="20">
-        <f t="shared" ref="D34:D65" si="3">SUM(B34:C34)</f>
+        <f t="shared" ref="D34:D50" si="3">SUM(B34:C34)</f>
         <v>0</v>
       </c>
       <c r="E34" s="32">
@@ -4030,7 +5201,7 @@
         <v>0</v>
       </c>
       <c r="F34" s="19">
-        <f t="shared" ref="F34:F65" si="4">SUM(D34:E34)</f>
+        <f t="shared" ref="F34:F50" si="4">SUM(D34:E34)</f>
         <v>0</v>
       </c>
       <c r="G34" s="32">
@@ -4038,7 +5209,7 @@
         <v>0</v>
       </c>
       <c r="H34" s="19">
-        <f t="shared" ref="H34:H65" si="5">SUM(F34:G34)</f>
+        <f t="shared" ref="H34:H50" si="5">SUM(F34:G34)</f>
         <v>0</v>
       </c>
     </row>
@@ -4659,11 +5830,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection sqref="A1:F17"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4989,10 +6160,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -5746,4 +6917,1704 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="2.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.9296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="107.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.86328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B1" s="71" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="71" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="71" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="71" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="71" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="71">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2">
+        <v>5.88</v>
+      </c>
+      <c r="D2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="71">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3">
+        <v>8.36</v>
+      </c>
+      <c r="D3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="71">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4">
+        <v>8.9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="71">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5">
+        <v>2.1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="71">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6">
+        <v>2.98</v>
+      </c>
+      <c r="D6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" t="s">
+        <v>104</v>
+      </c>
+      <c r="F6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="71">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="D7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="71">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8">
+        <v>2.29</v>
+      </c>
+      <c r="D8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="71">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="71">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10">
+        <v>1.6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" t="s">
+        <v>108</v>
+      </c>
+      <c r="F10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="71">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11">
+        <v>84.99</v>
+      </c>
+      <c r="D11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" s="71">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12">
+        <v>158</v>
+      </c>
+      <c r="D12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" s="71">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13">
+        <v>149</v>
+      </c>
+      <c r="D13" t="s">
+        <v>84</v>
+      </c>
+      <c r="E13" t="s">
+        <v>109</v>
+      </c>
+      <c r="F13" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" s="71">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14">
+        <v>279</v>
+      </c>
+      <c r="D14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" t="s">
+        <v>110</v>
+      </c>
+      <c r="F14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" s="71">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15">
+        <v>613.64</v>
+      </c>
+      <c r="D15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" t="s">
+        <v>70</v>
+      </c>
+      <c r="F15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" s="71">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16">
+        <v>425</v>
+      </c>
+      <c r="D16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" t="s">
+        <v>111</v>
+      </c>
+      <c r="F16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17" s="71">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17">
+        <v>145</v>
+      </c>
+      <c r="D17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" t="s">
+        <v>74</v>
+      </c>
+      <c r="F17" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:F48"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="2.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.9296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="119.1328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.86328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B1" s="71" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="71" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="71" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="71" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="71" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="71">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2">
+        <v>7.22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="71">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3">
+        <v>5.99</v>
+      </c>
+      <c r="D3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="71">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4">
+        <v>5.88</v>
+      </c>
+      <c r="D4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="71">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5">
+        <v>11.91</v>
+      </c>
+      <c r="D5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="71">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6">
+        <v>10.47</v>
+      </c>
+      <c r="D6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="71">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7">
+        <v>8.36</v>
+      </c>
+      <c r="D7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="71">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8">
+        <v>20.62</v>
+      </c>
+      <c r="D8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" t="s">
+        <v>112</v>
+      </c>
+      <c r="F8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="71">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9">
+        <v>17.55</v>
+      </c>
+      <c r="D9" t="s">
+        <v>87</v>
+      </c>
+      <c r="E9" t="s">
+        <v>113</v>
+      </c>
+      <c r="F9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="71">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10">
+        <v>8.9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" t="s">
+        <v>83</v>
+      </c>
+      <c r="F10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="71">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11">
+        <v>33.340000000000003</v>
+      </c>
+      <c r="D11" t="s">
+        <v>84</v>
+      </c>
+      <c r="E11" t="s">
+        <v>85</v>
+      </c>
+      <c r="F11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" s="71">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12">
+        <v>24.99</v>
+      </c>
+      <c r="D12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E12" t="s">
+        <v>115</v>
+      </c>
+      <c r="F12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" s="71">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13">
+        <v>3.98</v>
+      </c>
+      <c r="D13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F13" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" s="71">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14">
+        <v>5.99</v>
+      </c>
+      <c r="D14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" s="71">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15">
+        <v>2.1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>87</v>
+      </c>
+      <c r="E15" t="s">
+        <v>88</v>
+      </c>
+      <c r="F15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" s="71">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16">
+        <v>150</v>
+      </c>
+      <c r="D16" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" t="s">
+        <v>116</v>
+      </c>
+      <c r="F16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17" s="71">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17">
+        <v>5.99</v>
+      </c>
+      <c r="D17" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" t="s">
+        <v>117</v>
+      </c>
+      <c r="F17" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18" s="71">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18">
+        <v>2.98</v>
+      </c>
+      <c r="D18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" t="s">
+        <v>104</v>
+      </c>
+      <c r="F18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19" s="71">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19">
+        <v>2.98</v>
+      </c>
+      <c r="D19" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20" s="71">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="D20" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A21" s="71">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21">
+        <v>3.98</v>
+      </c>
+      <c r="D21" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" t="s">
+        <v>86</v>
+      </c>
+      <c r="F21" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A22" s="71">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22">
+        <v>5.99</v>
+      </c>
+      <c r="D22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" t="s">
+        <v>52</v>
+      </c>
+      <c r="F22" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23" s="71">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23">
+        <v>5.99</v>
+      </c>
+      <c r="D23" t="s">
+        <v>76</v>
+      </c>
+      <c r="E23" t="s">
+        <v>89</v>
+      </c>
+      <c r="F23" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24" s="71">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24">
+        <v>2.29</v>
+      </c>
+      <c r="D24" t="s">
+        <v>87</v>
+      </c>
+      <c r="E24" t="s">
+        <v>88</v>
+      </c>
+      <c r="F24" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25" s="71">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D25" t="s">
+        <v>57</v>
+      </c>
+      <c r="E25" t="s">
+        <v>106</v>
+      </c>
+      <c r="F25" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A26" s="71">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>105</v>
+      </c>
+      <c r="C26">
+        <v>5.99</v>
+      </c>
+      <c r="D26" t="s">
+        <v>76</v>
+      </c>
+      <c r="E26" t="s">
+        <v>118</v>
+      </c>
+      <c r="F26" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A27" s="71">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>107</v>
+      </c>
+      <c r="C27">
+        <v>1.6</v>
+      </c>
+      <c r="D27" t="s">
+        <v>57</v>
+      </c>
+      <c r="E27" t="s">
+        <v>108</v>
+      </c>
+      <c r="F27" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A28" s="71">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28">
+        <v>114</v>
+      </c>
+      <c r="D28" t="s">
+        <v>49</v>
+      </c>
+      <c r="E28" t="s">
+        <v>90</v>
+      </c>
+      <c r="F28" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29" s="71">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29">
+        <v>111.99</v>
+      </c>
+      <c r="D29" t="s">
+        <v>65</v>
+      </c>
+      <c r="E29" t="s">
+        <v>119</v>
+      </c>
+      <c r="F29" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A30" s="71">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30">
+        <v>84.99</v>
+      </c>
+      <c r="D30" t="s">
+        <v>120</v>
+      </c>
+      <c r="E30" t="s">
+        <v>121</v>
+      </c>
+      <c r="F30" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A31" s="71">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31">
+        <v>158</v>
+      </c>
+      <c r="D31" t="s">
+        <v>57</v>
+      </c>
+      <c r="E31" t="s">
+        <v>63</v>
+      </c>
+      <c r="F31" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A32" s="71">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32">
+        <v>159</v>
+      </c>
+      <c r="D32" t="s">
+        <v>76</v>
+      </c>
+      <c r="E32" t="s">
+        <v>93</v>
+      </c>
+      <c r="F32" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A33" s="71">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33">
+        <v>149</v>
+      </c>
+      <c r="D33" t="s">
+        <v>57</v>
+      </c>
+      <c r="E33" t="s">
+        <v>94</v>
+      </c>
+      <c r="F33" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A34" s="71">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34">
+        <v>149</v>
+      </c>
+      <c r="D34" t="s">
+        <v>76</v>
+      </c>
+      <c r="E34" t="s">
+        <v>122</v>
+      </c>
+      <c r="F34" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A35" s="71">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C35">
+        <v>200.02</v>
+      </c>
+      <c r="D35" t="s">
+        <v>84</v>
+      </c>
+      <c r="E35" t="s">
+        <v>109</v>
+      </c>
+      <c r="F35" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A36" s="71">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>67</v>
+      </c>
+      <c r="C36">
+        <v>289</v>
+      </c>
+      <c r="D36" t="s">
+        <v>57</v>
+      </c>
+      <c r="E36" t="s">
+        <v>68</v>
+      </c>
+      <c r="F36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A37" s="71">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37">
+        <v>279</v>
+      </c>
+      <c r="D37" t="s">
+        <v>76</v>
+      </c>
+      <c r="E37" t="s">
+        <v>95</v>
+      </c>
+      <c r="F37" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A38" s="71">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>67</v>
+      </c>
+      <c r="C38">
+        <v>315.01</v>
+      </c>
+      <c r="D38" t="s">
+        <v>65</v>
+      </c>
+      <c r="E38" t="s">
+        <v>110</v>
+      </c>
+      <c r="F38" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A39" s="71">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>67</v>
+      </c>
+      <c r="C39">
+        <v>339.09</v>
+      </c>
+      <c r="D39" t="s">
+        <v>96</v>
+      </c>
+      <c r="E39" t="s">
+        <v>97</v>
+      </c>
+      <c r="F39" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A40" s="71">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>69</v>
+      </c>
+      <c r="C40">
+        <v>765</v>
+      </c>
+      <c r="D40" t="s">
+        <v>57</v>
+      </c>
+      <c r="E40" t="s">
+        <v>98</v>
+      </c>
+      <c r="F40" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A41" s="71">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>69</v>
+      </c>
+      <c r="C41">
+        <v>613.64</v>
+      </c>
+      <c r="D41" t="s">
+        <v>49</v>
+      </c>
+      <c r="E41" t="s">
+        <v>70</v>
+      </c>
+      <c r="F41" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A42" s="71">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>69</v>
+      </c>
+      <c r="C42">
+        <v>1047.78</v>
+      </c>
+      <c r="D42" t="s">
+        <v>65</v>
+      </c>
+      <c r="E42" t="s">
+        <v>99</v>
+      </c>
+      <c r="F42" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A43" s="71">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>71</v>
+      </c>
+      <c r="C43">
+        <v>425</v>
+      </c>
+      <c r="D43" t="s">
+        <v>57</v>
+      </c>
+      <c r="E43" t="s">
+        <v>123</v>
+      </c>
+      <c r="F43" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A44" s="71">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>71</v>
+      </c>
+      <c r="C44">
+        <v>470.43</v>
+      </c>
+      <c r="D44" t="s">
+        <v>49</v>
+      </c>
+      <c r="E44" t="s">
+        <v>111</v>
+      </c>
+      <c r="F44" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A45" s="71">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>71</v>
+      </c>
+      <c r="C45">
+        <v>445.81</v>
+      </c>
+      <c r="D45" t="s">
+        <v>65</v>
+      </c>
+      <c r="E45" t="s">
+        <v>72</v>
+      </c>
+      <c r="F45" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A46" s="71">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>73</v>
+      </c>
+      <c r="C46">
+        <v>145</v>
+      </c>
+      <c r="D46" t="s">
+        <v>57</v>
+      </c>
+      <c r="E46" t="s">
+        <v>100</v>
+      </c>
+      <c r="F46" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A47" s="71">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>73</v>
+      </c>
+      <c r="C47">
+        <v>155.99</v>
+      </c>
+      <c r="D47" t="s">
+        <v>49</v>
+      </c>
+      <c r="E47" t="s">
+        <v>74</v>
+      </c>
+      <c r="F47" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A48" s="71">
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
+        <v>73</v>
+      </c>
+      <c r="C48">
+        <v>398.95</v>
+      </c>
+      <c r="D48" t="s">
+        <v>101</v>
+      </c>
+      <c r="E48" t="s">
+        <v>102</v>
+      </c>
+      <c r="F48" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="2.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.9296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="102.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.86328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B1" s="72" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="72" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="72" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="72" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="72">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2">
+        <v>5.88</v>
+      </c>
+      <c r="D2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="72">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3">
+        <v>8.36</v>
+      </c>
+      <c r="D3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="72">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4">
+        <v>8.9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" t="s">
+        <v>112</v>
+      </c>
+      <c r="F4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="72">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5">
+        <v>2.1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="72">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6">
+        <v>2.98</v>
+      </c>
+      <c r="D6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" t="s">
+        <v>104</v>
+      </c>
+      <c r="F6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="72">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="D7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="72">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8">
+        <v>2.29</v>
+      </c>
+      <c r="D8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="72">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="72">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10">
+        <v>1.6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" t="s">
+        <v>108</v>
+      </c>
+      <c r="F10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="72">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11">
+        <v>84.99</v>
+      </c>
+      <c r="D11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" s="72">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12">
+        <v>158</v>
+      </c>
+      <c r="D12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" s="72">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13">
+        <v>149</v>
+      </c>
+      <c r="D13" t="s">
+        <v>84</v>
+      </c>
+      <c r="E13" t="s">
+        <v>109</v>
+      </c>
+      <c r="F13" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" s="72">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14">
+        <v>279</v>
+      </c>
+      <c r="D14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" t="s">
+        <v>110</v>
+      </c>
+      <c r="F14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" s="72">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15">
+        <v>613.64</v>
+      </c>
+      <c r="D15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" t="s">
+        <v>70</v>
+      </c>
+      <c r="F15" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" s="72">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16">
+        <v>379</v>
+      </c>
+      <c r="D16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" t="s">
+        <v>111</v>
+      </c>
+      <c r="F16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17" s="72">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17">
+        <v>145</v>
+      </c>
+      <c r="D17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" t="s">
+        <v>74</v>
+      </c>
+      <c r="F17" t="s">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated csv data, a way to automate (possibly), and game plan
</commit_message>
<xml_diff>
--- a/Estimator_Worksheet.xlsx
+++ b/Estimator_Worksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kijah\Documents\Data_Bootcamp\Estimator_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B749ACB-04EF-4FC5-9F0E-0E29FE778A61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4D42A129-B11D-43DC-A410-CE80419BB9EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6105" yWindow="-16320" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6105" yWindow="-16320" windowWidth="29040" windowHeight="15720" firstSheet="9" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary - Rates" sheetId="1" r:id="rId1"/>
@@ -23,8 +23,13 @@
     <sheet name="Cleaned_Data1" sheetId="8" r:id="rId8"/>
     <sheet name="Working_Table2" sheetId="9" r:id="rId9"/>
     <sheet name="Cleaned_Data2" sheetId="10" r:id="rId10"/>
+    <sheet name="Working_Table3" sheetId="11" r:id="rId11"/>
+    <sheet name="Cleaned_Data3" sheetId="12" r:id="rId12"/>
+    <sheet name="Working_Table4" sheetId="13" r:id="rId13"/>
+    <sheet name="Cleaned_Data4" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -42,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1300" uniqueCount="146">
   <si>
     <t>Sales Tax</t>
   </si>
@@ -432,6 +437,54 @@
   </si>
   <si>
     <t>https://www.homedepot.com/p/Southwire-250-ft-14-2-Romex-SIMpull-Solid-NM-B-W-G-Wire-28827469/202019377</t>
+  </si>
+  <si>
+    <t>10/25/2022 09:25:56</t>
+  </si>
+  <si>
+    <t>10/25/2022 09:25:57</t>
+  </si>
+  <si>
+    <t>menards</t>
+  </si>
+  <si>
+    <t>https://www.menards.com/main/electrical/conduit-conduit-fittings-raceways/conduit/wheatland-tube-company-emt-conduit/3651321/p-1444446524964-c-6423.htm</t>
+  </si>
+  <si>
+    <t>mecampbell</t>
+  </si>
+  <si>
+    <t>https://www.mecampbell.com/1-x-10-ft-emt-conduit-color-silver-galvanized-steel-electrical-metallic-tubing.html</t>
+  </si>
+  <si>
+    <t>socalelectric</t>
+  </si>
+  <si>
+    <t>https://www.socalelectric.com/products/250-ft-14-2-romex-simpull-solid-nm-b-w-g-wire</t>
+  </si>
+  <si>
+    <t>https://www.cooper-electric.com/product/detail/14990/wic-thhn-6-str-blk-500r</t>
+  </si>
+  <si>
+    <t>wireandcableyourway</t>
+  </si>
+  <si>
+    <t>https://www.wireandcableyourway.com/10-awg-thhn-stranded-wire-500ft-1000ft-or-2500ft-spool</t>
+  </si>
+  <si>
+    <t>10/26/2022 13:58:13</t>
+  </si>
+  <si>
+    <t>https://www.lowes.com/pd/Sigma-Electric-ProConnex-3-4-in-Set-Screw-Coupling-Electrical-Metal-Tubing-Compatible-Conduit-Fitting/1100265</t>
+  </si>
+  <si>
+    <t>https://www.supplyworks.com/Sku/202077144/halex-12-in-electrical-metallic-tube-emt-set-screw-connector-5-pack-051411232108-23210</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/b/14-2-Romex-Indiana-OTHER-Industrial-Wires-Cables/92078/bn_7022085018</t>
+  </si>
+  <si>
+    <t>https://www.homedepot.com/p/Cerrowire-500-ft-10-Gauge-Black-Stranded-Copper-THHN-Wire-112-3871J/202304645</t>
   </si>
 </sst>
 </file>
@@ -442,7 +495,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -608,6 +661,16 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -677,7 +740,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -962,12 +1025,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1093,6 +1186,12 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1473,7 +1572,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
@@ -2502,6 +2601,2636 @@
       </c>
       <c r="F51" t="s">
         <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="2.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.46484375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="105.9296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.9296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B1" s="73" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="73" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="73" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="73" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="73" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="73">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2">
+        <v>5.88</v>
+      </c>
+      <c r="D2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="73">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3">
+        <v>8.36</v>
+      </c>
+      <c r="D3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="73">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4">
+        <v>8.9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" t="s">
+        <v>112</v>
+      </c>
+      <c r="F4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="73">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5">
+        <v>2.1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="73">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6">
+        <v>2.98</v>
+      </c>
+      <c r="D6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" t="s">
+        <v>104</v>
+      </c>
+      <c r="F6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="73">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="D7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="73">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8">
+        <v>3.98</v>
+      </c>
+      <c r="D8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="73">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="73">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10">
+        <v>1.6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" t="s">
+        <v>108</v>
+      </c>
+      <c r="F10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="73">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11">
+        <v>84.99</v>
+      </c>
+      <c r="D11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" s="73">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12">
+        <v>158</v>
+      </c>
+      <c r="D12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" s="73">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13">
+        <v>149</v>
+      </c>
+      <c r="D13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" t="s">
+        <v>94</v>
+      </c>
+      <c r="F13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" s="73">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14">
+        <v>289</v>
+      </c>
+      <c r="D14" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" t="s">
+        <v>68</v>
+      </c>
+      <c r="F14" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" s="73">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15">
+        <v>613.64</v>
+      </c>
+      <c r="D15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" t="s">
+        <v>70</v>
+      </c>
+      <c r="F15" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" s="73">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16">
+        <v>379</v>
+      </c>
+      <c r="D16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" t="s">
+        <v>111</v>
+      </c>
+      <c r="F16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17" s="73">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17">
+        <v>145</v>
+      </c>
+      <c r="D17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" t="s">
+        <v>74</v>
+      </c>
+      <c r="F17" t="s">
+        <v>131</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <dimension ref="A1:F49"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="2.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="142.06640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.9296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B1" s="73" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="73" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="73" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="73" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="73" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="73">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2">
+        <v>7.63</v>
+      </c>
+      <c r="D2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="73">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3">
+        <v>5.99</v>
+      </c>
+      <c r="D3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="73">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4">
+        <v>5.88</v>
+      </c>
+      <c r="D4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="73">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5">
+        <v>7.24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>132</v>
+      </c>
+      <c r="E5" t="s">
+        <v>133</v>
+      </c>
+      <c r="F5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="73">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6">
+        <v>11.91</v>
+      </c>
+      <c r="D6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="73">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7">
+        <v>10.47</v>
+      </c>
+      <c r="D7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="73">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8">
+        <v>8.36</v>
+      </c>
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="73">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9">
+        <v>98.99</v>
+      </c>
+      <c r="D9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="73">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10">
+        <v>20.62</v>
+      </c>
+      <c r="D10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" t="s">
+        <v>112</v>
+      </c>
+      <c r="F10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="73">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11">
+        <v>17.55</v>
+      </c>
+      <c r="D11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E11" t="s">
+        <v>113</v>
+      </c>
+      <c r="F11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" s="73">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12">
+        <v>8.9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>82</v>
+      </c>
+      <c r="E12" t="s">
+        <v>83</v>
+      </c>
+      <c r="F12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" s="73">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13">
+        <v>24.99</v>
+      </c>
+      <c r="D13" t="s">
+        <v>114</v>
+      </c>
+      <c r="E13" t="s">
+        <v>115</v>
+      </c>
+      <c r="F13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" s="73">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14">
+        <v>100</v>
+      </c>
+      <c r="D14" t="s">
+        <v>134</v>
+      </c>
+      <c r="E14" t="s">
+        <v>135</v>
+      </c>
+      <c r="F14" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" s="73">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15">
+        <v>3.98</v>
+      </c>
+      <c r="D15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" t="s">
+        <v>86</v>
+      </c>
+      <c r="F15" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" s="73">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16">
+        <v>5.99</v>
+      </c>
+      <c r="D16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17" s="73">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17">
+        <v>2.1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>87</v>
+      </c>
+      <c r="E17" t="s">
+        <v>88</v>
+      </c>
+      <c r="F17" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18" s="73">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18">
+        <v>5.99</v>
+      </c>
+      <c r="D18" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18" t="s">
+        <v>117</v>
+      </c>
+      <c r="F18" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19" s="73">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19">
+        <v>2.98</v>
+      </c>
+      <c r="D19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" t="s">
+        <v>104</v>
+      </c>
+      <c r="F19" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20" s="73">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20">
+        <v>3.66</v>
+      </c>
+      <c r="D20" t="s">
+        <v>78</v>
+      </c>
+      <c r="E20" t="s">
+        <v>126</v>
+      </c>
+      <c r="F20" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A21" s="73">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21">
+        <v>2.98</v>
+      </c>
+      <c r="D21" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" t="s">
+        <v>55</v>
+      </c>
+      <c r="F21" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A22" s="73">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22">
+        <v>3.6</v>
+      </c>
+      <c r="D22" t="s">
+        <v>127</v>
+      </c>
+      <c r="E22" t="s">
+        <v>128</v>
+      </c>
+      <c r="F22" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23" s="73">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="D23" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F23" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24" s="73">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24">
+        <v>3.98</v>
+      </c>
+      <c r="D24" t="s">
+        <v>57</v>
+      </c>
+      <c r="E24" t="s">
+        <v>86</v>
+      </c>
+      <c r="F24" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25" s="73">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25">
+        <v>5.99</v>
+      </c>
+      <c r="D25" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" t="s">
+        <v>52</v>
+      </c>
+      <c r="F25" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A26" s="73">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26">
+        <v>5.99</v>
+      </c>
+      <c r="D26" t="s">
+        <v>76</v>
+      </c>
+      <c r="E26" t="s">
+        <v>89</v>
+      </c>
+      <c r="F26" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A27" s="73">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>105</v>
+      </c>
+      <c r="C27">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D27" t="s">
+        <v>57</v>
+      </c>
+      <c r="E27" t="s">
+        <v>106</v>
+      </c>
+      <c r="F27" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A28" s="73">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>105</v>
+      </c>
+      <c r="C28">
+        <v>5.99</v>
+      </c>
+      <c r="D28" t="s">
+        <v>76</v>
+      </c>
+      <c r="E28" t="s">
+        <v>118</v>
+      </c>
+      <c r="F28" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29" s="73">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>107</v>
+      </c>
+      <c r="C29">
+        <v>1.6</v>
+      </c>
+      <c r="D29" t="s">
+        <v>57</v>
+      </c>
+      <c r="E29" t="s">
+        <v>108</v>
+      </c>
+      <c r="F29" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A30" s="73">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30">
+        <v>118</v>
+      </c>
+      <c r="D30" t="s">
+        <v>57</v>
+      </c>
+      <c r="E30" t="s">
+        <v>129</v>
+      </c>
+      <c r="F30" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A31" s="73">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31">
+        <v>114</v>
+      </c>
+      <c r="D31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E31" t="s">
+        <v>90</v>
+      </c>
+      <c r="F31" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A32" s="73">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32">
+        <v>111.99</v>
+      </c>
+      <c r="D32" t="s">
+        <v>65</v>
+      </c>
+      <c r="E32" t="s">
+        <v>119</v>
+      </c>
+      <c r="F32" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A33" s="73">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33">
+        <v>84.99</v>
+      </c>
+      <c r="D33" t="s">
+        <v>120</v>
+      </c>
+      <c r="E33" t="s">
+        <v>121</v>
+      </c>
+      <c r="F33" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A34" s="73">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34">
+        <v>117</v>
+      </c>
+      <c r="D34" t="s">
+        <v>136</v>
+      </c>
+      <c r="E34" t="s">
+        <v>137</v>
+      </c>
+      <c r="F34" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A35" s="73">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35">
+        <v>158</v>
+      </c>
+      <c r="D35" t="s">
+        <v>57</v>
+      </c>
+      <c r="E35" t="s">
+        <v>63</v>
+      </c>
+      <c r="F35" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A36" s="73">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36">
+        <v>159</v>
+      </c>
+      <c r="D36" t="s">
+        <v>76</v>
+      </c>
+      <c r="E36" t="s">
+        <v>93</v>
+      </c>
+      <c r="F36" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A37" s="73">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>64</v>
+      </c>
+      <c r="C37">
+        <v>149</v>
+      </c>
+      <c r="D37" t="s">
+        <v>57</v>
+      </c>
+      <c r="E37" t="s">
+        <v>94</v>
+      </c>
+      <c r="F37" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A38" s="73">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>67</v>
+      </c>
+      <c r="C38">
+        <v>289</v>
+      </c>
+      <c r="D38" t="s">
+        <v>57</v>
+      </c>
+      <c r="E38" t="s">
+        <v>68</v>
+      </c>
+      <c r="F38" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A39" s="73">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>67</v>
+      </c>
+      <c r="C39">
+        <v>289</v>
+      </c>
+      <c r="D39" t="s">
+        <v>76</v>
+      </c>
+      <c r="E39" t="s">
+        <v>95</v>
+      </c>
+      <c r="F39" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A40" s="73">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>67</v>
+      </c>
+      <c r="C40">
+        <v>339.09</v>
+      </c>
+      <c r="D40" t="s">
+        <v>96</v>
+      </c>
+      <c r="E40" t="s">
+        <v>97</v>
+      </c>
+      <c r="F40" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A41" s="73">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>69</v>
+      </c>
+      <c r="C41">
+        <v>613.64</v>
+      </c>
+      <c r="D41" t="s">
+        <v>49</v>
+      </c>
+      <c r="E41" t="s">
+        <v>70</v>
+      </c>
+      <c r="F41" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A42" s="73">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>69</v>
+      </c>
+      <c r="C42">
+        <v>1047.78</v>
+      </c>
+      <c r="D42" t="s">
+        <v>65</v>
+      </c>
+      <c r="E42" t="s">
+        <v>99</v>
+      </c>
+      <c r="F42" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A43" s="73">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>71</v>
+      </c>
+      <c r="C43">
+        <v>379</v>
+      </c>
+      <c r="D43" t="s">
+        <v>57</v>
+      </c>
+      <c r="E43" t="s">
+        <v>123</v>
+      </c>
+      <c r="F43" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A44" s="73">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>71</v>
+      </c>
+      <c r="C44">
+        <v>470.43</v>
+      </c>
+      <c r="D44" t="s">
+        <v>49</v>
+      </c>
+      <c r="E44" t="s">
+        <v>111</v>
+      </c>
+      <c r="F44" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A45" s="73">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>71</v>
+      </c>
+      <c r="C45">
+        <v>445.81</v>
+      </c>
+      <c r="D45" t="s">
+        <v>65</v>
+      </c>
+      <c r="E45" t="s">
+        <v>72</v>
+      </c>
+      <c r="F45" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A46" s="73">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>71</v>
+      </c>
+      <c r="C46">
+        <v>1144.69</v>
+      </c>
+      <c r="D46" t="s">
+        <v>101</v>
+      </c>
+      <c r="E46" t="s">
+        <v>138</v>
+      </c>
+      <c r="F46" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A47" s="73">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>73</v>
+      </c>
+      <c r="C47">
+        <v>145</v>
+      </c>
+      <c r="D47" t="s">
+        <v>57</v>
+      </c>
+      <c r="E47" t="s">
+        <v>100</v>
+      </c>
+      <c r="F47" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A48" s="73">
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
+        <v>73</v>
+      </c>
+      <c r="C48">
+        <v>155.99</v>
+      </c>
+      <c r="D48" t="s">
+        <v>49</v>
+      </c>
+      <c r="E48" t="s">
+        <v>74</v>
+      </c>
+      <c r="F48" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A49" s="73">
+        <v>47</v>
+      </c>
+      <c r="B49" t="s">
+        <v>73</v>
+      </c>
+      <c r="C49">
+        <v>165</v>
+      </c>
+      <c r="D49" t="s">
+        <v>139</v>
+      </c>
+      <c r="E49" t="s">
+        <v>140</v>
+      </c>
+      <c r="F49" t="s">
+        <v>131</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="2.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="114.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.9296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B1" s="74" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="74" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="74" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="74" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="74" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="74">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2">
+        <v>4.59</v>
+      </c>
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="74">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3">
+        <v>8.36</v>
+      </c>
+      <c r="D3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="74">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4">
+        <v>8.9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="74">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5">
+        <v>2.1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="74">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6">
+        <v>2.98</v>
+      </c>
+      <c r="D6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" t="s">
+        <v>104</v>
+      </c>
+      <c r="F6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="74">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="74">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8">
+        <v>3.98</v>
+      </c>
+      <c r="D8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="74">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="74">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10">
+        <v>1.6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" t="s">
+        <v>108</v>
+      </c>
+      <c r="F10" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="74">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11">
+        <v>84.99</v>
+      </c>
+      <c r="D11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" s="74">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12">
+        <v>159</v>
+      </c>
+      <c r="D12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" s="74">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13">
+        <v>149</v>
+      </c>
+      <c r="D13" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" t="s">
+        <v>94</v>
+      </c>
+      <c r="F13" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" s="74">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14">
+        <v>289</v>
+      </c>
+      <c r="D14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" t="s">
+        <v>110</v>
+      </c>
+      <c r="F14" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" s="74">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15">
+        <v>613.64</v>
+      </c>
+      <c r="D15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" t="s">
+        <v>70</v>
+      </c>
+      <c r="F15" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" s="74">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17" s="74">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17">
+        <v>145</v>
+      </c>
+      <c r="D17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" t="s">
+        <v>74</v>
+      </c>
+      <c r="F17" t="s">
+        <v>141</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <dimension ref="A1:F46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="2.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="127.265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.9296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B1" s="74" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="74" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="74" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="74" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="74" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="74">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2">
+        <v>7.22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="74">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3">
+        <v>5.99</v>
+      </c>
+      <c r="D3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="74">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4">
+        <v>4.59</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="74">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5">
+        <v>5.88</v>
+      </c>
+      <c r="D5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="74">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6">
+        <v>11.91</v>
+      </c>
+      <c r="D6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" t="s">
+        <v>80</v>
+      </c>
+      <c r="F6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="74">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7">
+        <v>10.47</v>
+      </c>
+      <c r="D7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="74">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8">
+        <v>8.36</v>
+      </c>
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="74">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9">
+        <v>98.99</v>
+      </c>
+      <c r="D9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="74">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10">
+        <v>20.62</v>
+      </c>
+      <c r="D10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" t="s">
+        <v>112</v>
+      </c>
+      <c r="F10" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="74">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11">
+        <v>17.55</v>
+      </c>
+      <c r="D11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E11" t="s">
+        <v>113</v>
+      </c>
+      <c r="F11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" s="74">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12">
+        <v>8.9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>82</v>
+      </c>
+      <c r="E12" t="s">
+        <v>83</v>
+      </c>
+      <c r="F12" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" s="74">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13">
+        <v>33.340000000000003</v>
+      </c>
+      <c r="D13" t="s">
+        <v>84</v>
+      </c>
+      <c r="E13" t="s">
+        <v>85</v>
+      </c>
+      <c r="F13" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" s="74">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14">
+        <v>24.99</v>
+      </c>
+      <c r="D14" t="s">
+        <v>114</v>
+      </c>
+      <c r="E14" t="s">
+        <v>115</v>
+      </c>
+      <c r="F14" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" s="74">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15">
+        <v>100</v>
+      </c>
+      <c r="D15" t="s">
+        <v>134</v>
+      </c>
+      <c r="E15" t="s">
+        <v>135</v>
+      </c>
+      <c r="F15" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" s="74">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16">
+        <v>3.98</v>
+      </c>
+      <c r="D16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" t="s">
+        <v>86</v>
+      </c>
+      <c r="F16" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17" s="74">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17">
+        <v>5.99</v>
+      </c>
+      <c r="D17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A18" s="74">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18">
+        <v>2.1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>87</v>
+      </c>
+      <c r="E18" t="s">
+        <v>88</v>
+      </c>
+      <c r="F18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A19" s="74">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19">
+        <v>5.99</v>
+      </c>
+      <c r="D19" t="s">
+        <v>76</v>
+      </c>
+      <c r="E19" t="s">
+        <v>117</v>
+      </c>
+      <c r="F19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A20" s="74">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20">
+        <v>2.98</v>
+      </c>
+      <c r="D20" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" t="s">
+        <v>104</v>
+      </c>
+      <c r="F20" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A21" s="74">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21">
+        <v>3.66</v>
+      </c>
+      <c r="D21" t="s">
+        <v>78</v>
+      </c>
+      <c r="E21" t="s">
+        <v>126</v>
+      </c>
+      <c r="F21" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A22" s="74">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22">
+        <v>5.99</v>
+      </c>
+      <c r="D22" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22" t="s">
+        <v>142</v>
+      </c>
+      <c r="F22" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23" s="74">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23">
+        <v>2.98</v>
+      </c>
+      <c r="D23" t="s">
+        <v>54</v>
+      </c>
+      <c r="E23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F23" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24" s="74">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24">
+        <v>3.98</v>
+      </c>
+      <c r="D24" t="s">
+        <v>57</v>
+      </c>
+      <c r="E24" t="s">
+        <v>86</v>
+      </c>
+      <c r="F24" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25" s="74">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25">
+        <v>5.99</v>
+      </c>
+      <c r="D25" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" t="s">
+        <v>52</v>
+      </c>
+      <c r="F25" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A26" s="74">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26">
+        <v>5.99</v>
+      </c>
+      <c r="D26" t="s">
+        <v>76</v>
+      </c>
+      <c r="E26" t="s">
+        <v>89</v>
+      </c>
+      <c r="F26" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A27" s="74">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27">
+        <v>150</v>
+      </c>
+      <c r="D27" t="s">
+        <v>78</v>
+      </c>
+      <c r="E27" t="s">
+        <v>143</v>
+      </c>
+      <c r="F27" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A28" s="74">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>105</v>
+      </c>
+      <c r="C28">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="D28" t="s">
+        <v>57</v>
+      </c>
+      <c r="E28" t="s">
+        <v>106</v>
+      </c>
+      <c r="F28" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29" s="74">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>105</v>
+      </c>
+      <c r="C29">
+        <v>5.99</v>
+      </c>
+      <c r="D29" t="s">
+        <v>76</v>
+      </c>
+      <c r="E29" t="s">
+        <v>118</v>
+      </c>
+      <c r="F29" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A30" s="74">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>107</v>
+      </c>
+      <c r="C30">
+        <v>1.6</v>
+      </c>
+      <c r="D30" t="s">
+        <v>57</v>
+      </c>
+      <c r="E30" t="s">
+        <v>108</v>
+      </c>
+      <c r="F30" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A31" s="74">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31">
+        <v>114</v>
+      </c>
+      <c r="D31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E31" t="s">
+        <v>90</v>
+      </c>
+      <c r="F31" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A32" s="74">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32">
+        <v>111.07</v>
+      </c>
+      <c r="D32" t="s">
+        <v>65</v>
+      </c>
+      <c r="E32" t="s">
+        <v>144</v>
+      </c>
+      <c r="F32" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A33" s="74">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33">
+        <v>117</v>
+      </c>
+      <c r="D33" t="s">
+        <v>136</v>
+      </c>
+      <c r="E33" t="s">
+        <v>137</v>
+      </c>
+      <c r="F33" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A34" s="74">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34">
+        <v>84.99</v>
+      </c>
+      <c r="D34" t="s">
+        <v>120</v>
+      </c>
+      <c r="E34" t="s">
+        <v>121</v>
+      </c>
+      <c r="F34" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A35" s="74">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35">
+        <v>159</v>
+      </c>
+      <c r="D35" t="s">
+        <v>57</v>
+      </c>
+      <c r="E35" t="s">
+        <v>63</v>
+      </c>
+      <c r="F35" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A36" s="74">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36">
+        <v>159</v>
+      </c>
+      <c r="D36" t="s">
+        <v>76</v>
+      </c>
+      <c r="E36" t="s">
+        <v>93</v>
+      </c>
+      <c r="F36" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A37" s="74">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>64</v>
+      </c>
+      <c r="C37">
+        <v>149</v>
+      </c>
+      <c r="D37" t="s">
+        <v>57</v>
+      </c>
+      <c r="E37" t="s">
+        <v>94</v>
+      </c>
+      <c r="F37" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A38" s="74">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>67</v>
+      </c>
+      <c r="C38">
+        <v>289</v>
+      </c>
+      <c r="D38" t="s">
+        <v>57</v>
+      </c>
+      <c r="E38" t="s">
+        <v>68</v>
+      </c>
+      <c r="F38" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A39" s="74">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>67</v>
+      </c>
+      <c r="C39">
+        <v>289</v>
+      </c>
+      <c r="D39" t="s">
+        <v>76</v>
+      </c>
+      <c r="E39" t="s">
+        <v>95</v>
+      </c>
+      <c r="F39" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A40" s="74">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>67</v>
+      </c>
+      <c r="C40">
+        <v>315.01</v>
+      </c>
+      <c r="D40" t="s">
+        <v>65</v>
+      </c>
+      <c r="E40" t="s">
+        <v>110</v>
+      </c>
+      <c r="F40" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A41" s="74">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>69</v>
+      </c>
+      <c r="C41">
+        <v>613.64</v>
+      </c>
+      <c r="D41" t="s">
+        <v>49</v>
+      </c>
+      <c r="E41" t="s">
+        <v>70</v>
+      </c>
+      <c r="F41" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A42" s="74">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>69</v>
+      </c>
+      <c r="C42">
+        <v>1047.78</v>
+      </c>
+      <c r="D42" t="s">
+        <v>65</v>
+      </c>
+      <c r="E42" t="s">
+        <v>99</v>
+      </c>
+      <c r="F42" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A43" s="74">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>73</v>
+      </c>
+      <c r="C43">
+        <v>145</v>
+      </c>
+      <c r="D43" t="s">
+        <v>57</v>
+      </c>
+      <c r="E43" t="s">
+        <v>100</v>
+      </c>
+      <c r="F43" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A44" s="74">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>73</v>
+      </c>
+      <c r="C44">
+        <v>145</v>
+      </c>
+      <c r="D44" t="s">
+        <v>57</v>
+      </c>
+      <c r="E44" t="s">
+        <v>145</v>
+      </c>
+      <c r="F44" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A45" s="74">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>73</v>
+      </c>
+      <c r="C45">
+        <v>155.99</v>
+      </c>
+      <c r="D45" t="s">
+        <v>49</v>
+      </c>
+      <c r="E45" t="s">
+        <v>74</v>
+      </c>
+      <c r="F45" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A46" s="74">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>73</v>
+      </c>
+      <c r="C46">
+        <v>165</v>
+      </c>
+      <c r="D46" t="s">
+        <v>139</v>
+      </c>
+      <c r="E46" t="s">
+        <v>140</v>
+      </c>
+      <c r="F46" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -2744,13 +5473,13 @@
       <c r="P8" s="63"/>
     </row>
     <row r="9" spans="1:16" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="73" t="s">
+      <c r="A9" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="74"/>
-      <c r="C9" s="74"/>
-      <c r="D9" s="74"/>
-      <c r="E9" s="75"/>
+      <c r="B9" s="76"/>
+      <c r="C9" s="76"/>
+      <c r="D9" s="76"/>
+      <c r="E9" s="77"/>
       <c r="F9" s="9"/>
       <c r="G9" s="51">
         <f t="shared" si="1"/>
@@ -2773,14 +5502,14 @@
         <v>11</v>
       </c>
       <c r="D10" s="14"/>
-      <c r="E10" s="76" t="s">
+      <c r="E10" s="78" t="s">
         <v>12</v>
       </c>
       <c r="F10" s="54" t="str">
         <f>C10</f>
         <v>TOTAL</v>
       </c>
-      <c r="G10" s="78" t="s">
+      <c r="G10" s="80" t="s">
         <v>13</v>
       </c>
       <c r="H10" s="63"/>
@@ -2800,11 +5529,11 @@
         <v>14</v>
       </c>
       <c r="D11" s="55"/>
-      <c r="E11" s="77"/>
+      <c r="E11" s="79"/>
       <c r="F11" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="79"/>
+      <c r="G11" s="81"/>
       <c r="H11" s="63"/>
       <c r="I11" s="63"/>
       <c r="J11" s="63"/>
@@ -2816,59 +5545,59 @@
       <c r="P11" s="63"/>
     </row>
     <row r="12" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="80" t="s">
+      <c r="A12" s="82" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="81">
+      <c r="B12" s="83">
         <f t="shared" ref="B12:G12" si="2">SUM(B2:B8)</f>
         <v>0</v>
       </c>
-      <c r="C12" s="81">
+      <c r="C12" s="83">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="D12" s="81">
+      <c r="D12" s="83">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E12" s="81">
+      <c r="E12" s="83">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F12" s="81">
+      <c r="F12" s="83">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G12" s="84">
+      <c r="G12" s="86">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H12" s="86" t="s">
+      <c r="H12" s="88" t="s">
         <v>17</v>
       </c>
-      <c r="I12" s="79"/>
-      <c r="J12" s="79"/>
-      <c r="K12" s="79"/>
-      <c r="L12" s="79"/>
-      <c r="M12" s="79"/>
+      <c r="I12" s="81"/>
+      <c r="J12" s="81"/>
+      <c r="K12" s="81"/>
+      <c r="L12" s="81"/>
+      <c r="M12" s="81"/>
       <c r="N12" s="63"/>
       <c r="O12" s="63"/>
       <c r="P12" s="63"/>
     </row>
     <row r="13" spans="1:16" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="79"/>
-      <c r="B13" s="79"/>
-      <c r="C13" s="79"/>
-      <c r="D13" s="79"/>
-      <c r="E13" s="79"/>
-      <c r="F13" s="79"/>
-      <c r="G13" s="85"/>
-      <c r="H13" s="87"/>
-      <c r="I13" s="79"/>
-      <c r="J13" s="79"/>
-      <c r="K13" s="79"/>
-      <c r="L13" s="79"/>
-      <c r="M13" s="79"/>
+      <c r="A13" s="81"/>
+      <c r="B13" s="81"/>
+      <c r="C13" s="81"/>
+      <c r="D13" s="81"/>
+      <c r="E13" s="81"/>
+      <c r="F13" s="81"/>
+      <c r="G13" s="87"/>
+      <c r="H13" s="89"/>
+      <c r="I13" s="81"/>
+      <c r="J13" s="81"/>
+      <c r="K13" s="81"/>
+      <c r="L13" s="81"/>
+      <c r="M13" s="81"/>
       <c r="N13" s="63"/>
       <c r="O13" s="63"/>
       <c r="P13" s="63"/>
@@ -2933,10 +5662,10 @@
       <c r="B18" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="88"/>
-      <c r="D18" s="89"/>
-      <c r="E18" s="89"/>
-      <c r="F18" s="89"/>
+      <c r="C18" s="90"/>
+      <c r="D18" s="91"/>
+      <c r="E18" s="91"/>
+      <c r="F18" s="91"/>
       <c r="G18" s="63"/>
       <c r="H18" s="63"/>
       <c r="I18" s="63"/>
@@ -2953,10 +5682,10 @@
       <c r="B19" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="82"/>
-      <c r="D19" s="74"/>
-      <c r="E19" s="74"/>
-      <c r="F19" s="74"/>
+      <c r="C19" s="84"/>
+      <c r="D19" s="76"/>
+      <c r="E19" s="76"/>
+      <c r="F19" s="76"/>
       <c r="G19" s="63"/>
       <c r="H19" s="63"/>
       <c r="I19" s="63"/>
@@ -2973,15 +5702,15 @@
       <c r="B20" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="88"/>
-      <c r="D20" s="89"/>
-      <c r="E20" s="89"/>
-      <c r="F20" s="89"/>
-      <c r="G20" s="89"/>
-      <c r="H20" s="89"/>
-      <c r="I20" s="89"/>
-      <c r="J20" s="89"/>
-      <c r="K20" s="89"/>
+      <c r="C20" s="90"/>
+      <c r="D20" s="91"/>
+      <c r="E20" s="91"/>
+      <c r="F20" s="91"/>
+      <c r="G20" s="91"/>
+      <c r="H20" s="91"/>
+      <c r="I20" s="91"/>
+      <c r="J20" s="91"/>
+      <c r="K20" s="91"/>
       <c r="L20" s="63"/>
       <c r="M20" s="63"/>
       <c r="N20" s="63"/>
@@ -2993,10 +5722,10 @@
       <c r="B21" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="82"/>
-      <c r="D21" s="74"/>
-      <c r="E21" s="74"/>
-      <c r="F21" s="74"/>
+      <c r="C21" s="84"/>
+      <c r="D21" s="76"/>
+      <c r="E21" s="76"/>
+      <c r="F21" s="76"/>
       <c r="G21" s="67"/>
       <c r="H21" s="63"/>
       <c r="I21" s="63"/>
@@ -3026,14 +5755,14 @@
     <row r="23" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A23" s="63"/>
       <c r="B23" s="63"/>
-      <c r="C23" s="83" t="s">
+      <c r="C23" s="85" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="79"/>
-      <c r="E23" s="79"/>
-      <c r="F23" s="79"/>
-      <c r="G23" s="79"/>
-      <c r="H23" s="79"/>
+      <c r="D23" s="81"/>
+      <c r="E23" s="81"/>
+      <c r="F23" s="81"/>
+      <c r="G23" s="81"/>
+      <c r="H23" s="81"/>
       <c r="I23" s="63"/>
       <c r="J23" s="63"/>
       <c r="K23" s="63"/>
@@ -3046,12 +5775,12 @@
     <row r="24" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A24" s="63"/>
       <c r="B24" s="63"/>
-      <c r="C24" s="79"/>
-      <c r="D24" s="79"/>
-      <c r="E24" s="79"/>
-      <c r="F24" s="79"/>
-      <c r="G24" s="79"/>
-      <c r="H24" s="79"/>
+      <c r="C24" s="81"/>
+      <c r="D24" s="81"/>
+      <c r="E24" s="81"/>
+      <c r="F24" s="81"/>
+      <c r="G24" s="81"/>
+      <c r="H24" s="81"/>
       <c r="I24" s="63"/>
       <c r="J24" s="63"/>
       <c r="K24" s="63"/>
@@ -3064,12 +5793,12 @@
     <row r="25" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A25" s="63"/>
       <c r="B25" s="63"/>
-      <c r="C25" s="79"/>
-      <c r="D25" s="79"/>
-      <c r="E25" s="79"/>
-      <c r="F25" s="79"/>
-      <c r="G25" s="79"/>
-      <c r="H25" s="79"/>
+      <c r="C25" s="81"/>
+      <c r="D25" s="81"/>
+      <c r="E25" s="81"/>
+      <c r="F25" s="81"/>
+      <c r="G25" s="81"/>
+      <c r="H25" s="81"/>
       <c r="I25" s="63"/>
       <c r="J25" s="63"/>
       <c r="K25" s="63"/>
@@ -3728,11 +6457,11 @@
         <v>1</v>
       </c>
       <c r="F34" s="7">
-        <f t="shared" ref="F34:F50" si="2">B34*(C34/E34)</f>
+        <f t="shared" ref="F34:F65" si="2">B34*(C34/E34)</f>
         <v>0</v>
       </c>
       <c r="H34">
-        <f t="shared" ref="H34:H50" si="3">B34*(G34/E34)</f>
+        <f t="shared" ref="H34:H65" si="3">B34*(G34/E34)</f>
         <v>0</v>
       </c>
     </row>
@@ -5193,7 +7922,7 @@
         <v>0</v>
       </c>
       <c r="D34" s="20">
-        <f t="shared" ref="D34:D50" si="3">SUM(B34:C34)</f>
+        <f t="shared" ref="D34:D65" si="3">SUM(B34:C34)</f>
         <v>0</v>
       </c>
       <c r="E34" s="32">
@@ -5201,7 +7930,7 @@
         <v>0</v>
       </c>
       <c r="F34" s="19">
-        <f t="shared" ref="F34:F50" si="4">SUM(D34:E34)</f>
+        <f t="shared" ref="F34:F65" si="4">SUM(D34:E34)</f>
         <v>0</v>
       </c>
       <c r="G34" s="32">
@@ -5209,7 +7938,7 @@
         <v>0</v>
       </c>
       <c r="H34" s="19">
-        <f t="shared" ref="H34:H50" si="5">SUM(F34:G34)</f>
+        <f t="shared" ref="H34:H65" si="5">SUM(F34:G34)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>